<commit_message>
team filter data alphabetized
sort order was slightly off due to team codes getting precedence.
</commit_message>
<xml_diff>
--- a/filters/db/teams-by-league.xlsx
+++ b/filters/db/teams-by-league.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NCAA" sheetId="1" r:id="rId1"/>
@@ -4065,7 +4065,7 @@
   <dimension ref="A1:G222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:G3"/>
+      <selection activeCell="A4" sqref="A4:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4074,25 +4074,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -4107,7 +4107,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -4156,7 +4156,7 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -4179,7 +4179,7 @@
         <v>446</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G5">
         <v>150</v>
@@ -4225,7 +4225,7 @@
         <v>448</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G7">
         <v>150</v>
@@ -4302,7 +4302,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -4311,10 +4311,10 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F11" t="s">
         <v>644</v>
@@ -4325,7 +4325,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -4334,10 +4334,10 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F12" t="s">
         <v>644</v>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -4610,10 +4610,10 @@
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="F24" t="s">
         <v>644</v>
@@ -4624,7 +4624,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -4633,10 +4633,10 @@
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F25" t="s">
         <v>644</v>
@@ -4877,7 +4877,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>356</v>
       </c>
       <c r="B36" t="s">
         <v>8</v>
@@ -4886,10 +4886,10 @@
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>82</v>
+        <v>357</v>
       </c>
       <c r="E36" t="s">
-        <v>474</v>
+        <v>357</v>
       </c>
       <c r="F36" t="s">
         <v>644</v>
@@ -4900,7 +4900,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
         <v>8</v>
@@ -4909,10 +4909,10 @@
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E37" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F37" t="s">
         <v>644</v>
@@ -4923,7 +4923,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
@@ -4932,10 +4932,10 @@
         <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E38" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F38" t="s">
         <v>644</v>
@@ -4946,7 +4946,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
@@ -4955,10 +4955,10 @@
         <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E39" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F39" t="s">
         <v>644</v>
@@ -4969,7 +4969,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -4978,10 +4978,10 @@
         <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E40" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F40" t="s">
         <v>644</v>
@@ -4992,7 +4992,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -5001,10 +5001,10 @@
         <v>17</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E41" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F41" t="s">
         <v>644</v>
@@ -5015,7 +5015,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -5024,10 +5024,10 @@
         <v>17</v>
       </c>
       <c r="D42" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E42" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F42" t="s">
         <v>644</v>
@@ -5038,7 +5038,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -5047,10 +5047,10 @@
         <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E43" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F43" t="s">
         <v>644</v>
@@ -5061,7 +5061,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
         <v>8</v>
@@ -5070,10 +5070,10 @@
         <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E44" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F44" t="s">
         <v>644</v>
@@ -5084,7 +5084,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
@@ -5093,10 +5093,10 @@
         <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E45" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F45" t="s">
         <v>644</v>
@@ -5107,7 +5107,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
@@ -5116,10 +5116,10 @@
         <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E46" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F46" t="s">
         <v>644</v>
@@ -5130,7 +5130,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
@@ -5139,10 +5139,10 @@
         <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E47" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F47" t="s">
         <v>644</v>
@@ -5153,7 +5153,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
         <v>8</v>
@@ -5162,10 +5162,10 @@
         <v>17</v>
       </c>
       <c r="D48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E48" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F48" t="s">
         <v>644</v>
@@ -5176,7 +5176,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B49" t="s">
         <v>8</v>
@@ -5185,10 +5185,10 @@
         <v>17</v>
       </c>
       <c r="D49" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E49" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F49" t="s">
         <v>644</v>
@@ -5199,7 +5199,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
@@ -5208,10 +5208,10 @@
         <v>17</v>
       </c>
       <c r="D50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E50" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F50" t="s">
         <v>644</v>
@@ -5222,7 +5222,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
@@ -5231,10 +5231,10 @@
         <v>17</v>
       </c>
       <c r="D51" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E51" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F51" t="s">
         <v>644</v>
@@ -5245,7 +5245,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B52" t="s">
         <v>8</v>
@@ -5254,10 +5254,10 @@
         <v>17</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E52" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F52" t="s">
         <v>644</v>
@@ -5268,7 +5268,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
@@ -5277,10 +5277,10 @@
         <v>17</v>
       </c>
       <c r="D53" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E53" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F53" t="s">
         <v>644</v>
@@ -5291,7 +5291,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B54" t="s">
         <v>8</v>
@@ -5300,10 +5300,10 @@
         <v>17</v>
       </c>
       <c r="D54" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E54" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F54" t="s">
         <v>644</v>
@@ -5314,7 +5314,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
@@ -5323,10 +5323,10 @@
         <v>17</v>
       </c>
       <c r="D55" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E55" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F55" t="s">
         <v>644</v>
@@ -5337,7 +5337,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B56" t="s">
         <v>8</v>
@@ -5346,10 +5346,10 @@
         <v>17</v>
       </c>
       <c r="D56" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E56" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F56" t="s">
         <v>644</v>
@@ -5360,7 +5360,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B57" t="s">
         <v>8</v>
@@ -5369,10 +5369,10 @@
         <v>17</v>
       </c>
       <c r="D57" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E57" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F57" t="s">
         <v>644</v>
@@ -5383,7 +5383,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B58" t="s">
         <v>8</v>
@@ -5392,10 +5392,10 @@
         <v>17</v>
       </c>
       <c r="D58" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E58" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F58" t="s">
         <v>644</v>
@@ -5406,7 +5406,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B59" t="s">
         <v>8</v>
@@ -5415,10 +5415,10 @@
         <v>17</v>
       </c>
       <c r="D59" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E59" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F59" t="s">
         <v>644</v>
@@ -5429,7 +5429,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B60" t="s">
         <v>8</v>
@@ -5438,10 +5438,10 @@
         <v>17</v>
       </c>
       <c r="D60" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E60" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F60" t="s">
         <v>644</v>
@@ -5452,7 +5452,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B61" t="s">
         <v>8</v>
@@ -5461,10 +5461,10 @@
         <v>17</v>
       </c>
       <c r="D61" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E61" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F61" t="s">
         <v>644</v>
@@ -5475,7 +5475,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B62" t="s">
         <v>8</v>
@@ -5484,10 +5484,10 @@
         <v>17</v>
       </c>
       <c r="D62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E62" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F62" t="s">
         <v>644</v>
@@ -5498,7 +5498,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B63" t="s">
         <v>8</v>
@@ -5507,10 +5507,10 @@
         <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E63" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F63" t="s">
         <v>644</v>
@@ -5521,7 +5521,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B64" t="s">
         <v>8</v>
@@ -5530,10 +5530,10 @@
         <v>17</v>
       </c>
       <c r="D64" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E64" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F64" t="s">
         <v>644</v>
@@ -5544,7 +5544,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
@@ -5553,10 +5553,10 @@
         <v>17</v>
       </c>
       <c r="D65" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E65" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F65" t="s">
         <v>644</v>
@@ -5567,7 +5567,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B66" t="s">
         <v>8</v>
@@ -5576,10 +5576,10 @@
         <v>17</v>
       </c>
       <c r="D66" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E66" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F66" t="s">
         <v>644</v>
@@ -5590,7 +5590,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B67" t="s">
         <v>8</v>
@@ -5599,10 +5599,10 @@
         <v>17</v>
       </c>
       <c r="D67" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E67" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F67" t="s">
         <v>644</v>
@@ -5613,7 +5613,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B68" t="s">
         <v>8</v>
@@ -5622,10 +5622,10 @@
         <v>17</v>
       </c>
       <c r="D68" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E68" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F68" t="s">
         <v>644</v>
@@ -5636,7 +5636,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B69" t="s">
         <v>8</v>
@@ -5645,10 +5645,10 @@
         <v>17</v>
       </c>
       <c r="D69" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E69" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F69" t="s">
         <v>644</v>
@@ -5659,7 +5659,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B70" t="s">
         <v>8</v>
@@ -5668,10 +5668,10 @@
         <v>17</v>
       </c>
       <c r="D70" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E70" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F70" t="s">
         <v>644</v>
@@ -5682,7 +5682,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B71" t="s">
         <v>8</v>
@@ -5691,10 +5691,10 @@
         <v>17</v>
       </c>
       <c r="D71" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E71" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F71" t="s">
         <v>644</v>
@@ -5705,7 +5705,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B72" t="s">
         <v>8</v>
@@ -5714,10 +5714,10 @@
         <v>17</v>
       </c>
       <c r="D72" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E72" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F72" t="s">
         <v>644</v>
@@ -5728,7 +5728,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B73" t="s">
         <v>8</v>
@@ -5737,10 +5737,10 @@
         <v>17</v>
       </c>
       <c r="D73" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E73" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F73" t="s">
         <v>644</v>
@@ -5751,7 +5751,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B74" t="s">
         <v>8</v>
@@ -5760,10 +5760,10 @@
         <v>17</v>
       </c>
       <c r="D74" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E74" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F74" t="s">
         <v>644</v>
@@ -5774,7 +5774,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B75" t="s">
         <v>8</v>
@@ -5783,10 +5783,10 @@
         <v>17</v>
       </c>
       <c r="D75" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E75" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F75" t="s">
         <v>644</v>
@@ -5797,7 +5797,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B76" t="s">
         <v>8</v>
@@ -5806,10 +5806,10 @@
         <v>17</v>
       </c>
       <c r="D76" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E76" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F76" t="s">
         <v>644</v>
@@ -5820,7 +5820,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B77" t="s">
         <v>8</v>
@@ -5829,10 +5829,10 @@
         <v>17</v>
       </c>
       <c r="D77" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E77" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F77" t="s">
         <v>644</v>
@@ -5843,7 +5843,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B78" t="s">
         <v>8</v>
@@ -5852,10 +5852,10 @@
         <v>17</v>
       </c>
       <c r="D78" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E78" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F78" t="s">
         <v>644</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B79" t="s">
         <v>8</v>
@@ -5875,10 +5875,10 @@
         <v>17</v>
       </c>
       <c r="D79" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E79" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F79" t="s">
         <v>644</v>
@@ -5889,7 +5889,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B80" t="s">
         <v>8</v>
@@ -5898,10 +5898,10 @@
         <v>17</v>
       </c>
       <c r="D80" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E80" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F80" t="s">
         <v>644</v>
@@ -5912,7 +5912,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B81" t="s">
         <v>8</v>
@@ -5921,10 +5921,10 @@
         <v>17</v>
       </c>
       <c r="D81" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E81" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F81" t="s">
         <v>644</v>
@@ -5935,7 +5935,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B82" t="s">
         <v>8</v>
@@ -5944,10 +5944,10 @@
         <v>17</v>
       </c>
       <c r="D82" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E82" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F82" t="s">
         <v>644</v>
@@ -5958,7 +5958,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B83" t="s">
         <v>8</v>
@@ -5967,10 +5967,10 @@
         <v>17</v>
       </c>
       <c r="D83" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E83" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F83" t="s">
         <v>644</v>
@@ -5981,7 +5981,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B84" t="s">
         <v>8</v>
@@ -5990,10 +5990,10 @@
         <v>17</v>
       </c>
       <c r="D84" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E84" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F84" t="s">
         <v>644</v>
@@ -6004,7 +6004,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B85" t="s">
         <v>8</v>
@@ -6013,10 +6013,10 @@
         <v>17</v>
       </c>
       <c r="D85" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E85" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F85" t="s">
         <v>644</v>
@@ -6027,7 +6027,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B86" t="s">
         <v>8</v>
@@ -6036,10 +6036,10 @@
         <v>17</v>
       </c>
       <c r="D86" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E86" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F86" t="s">
         <v>644</v>
@@ -6050,7 +6050,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
@@ -6059,10 +6059,10 @@
         <v>17</v>
       </c>
       <c r="D87" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E87" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F87" t="s">
         <v>644</v>
@@ -6073,7 +6073,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B88" t="s">
         <v>8</v>
@@ -6082,10 +6082,10 @@
         <v>17</v>
       </c>
       <c r="D88" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E88" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F88" t="s">
         <v>644</v>
@@ -6096,7 +6096,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B89" t="s">
         <v>8</v>
@@ -6105,10 +6105,10 @@
         <v>17</v>
       </c>
       <c r="D89" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E89" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F89" t="s">
         <v>644</v>
@@ -6119,7 +6119,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B90" t="s">
         <v>8</v>
@@ -6128,10 +6128,10 @@
         <v>17</v>
       </c>
       <c r="D90" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E90" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F90" t="s">
         <v>644</v>
@@ -6142,7 +6142,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B91" t="s">
         <v>8</v>
@@ -6151,10 +6151,10 @@
         <v>17</v>
       </c>
       <c r="D91" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E91" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F91" t="s">
         <v>644</v>
@@ -6165,7 +6165,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B92" t="s">
         <v>8</v>
@@ -6177,7 +6177,7 @@
         <v>191</v>
       </c>
       <c r="E92" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F92" t="s">
         <v>644</v>
@@ -6188,7 +6188,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B93" t="s">
         <v>8</v>
@@ -6197,10 +6197,10 @@
         <v>17</v>
       </c>
       <c r="D93" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E93" t="s">
-        <v>194</v>
+        <v>530</v>
       </c>
       <c r="F93" t="s">
         <v>644</v>
@@ -6211,7 +6211,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B94" t="s">
         <v>8</v>
@@ -6220,10 +6220,10 @@
         <v>17</v>
       </c>
       <c r="D94" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E94" t="s">
-        <v>531</v>
+        <v>194</v>
       </c>
       <c r="F94" t="s">
         <v>644</v>
@@ -6234,7 +6234,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B95" t="s">
         <v>8</v>
@@ -6243,10 +6243,10 @@
         <v>17</v>
       </c>
       <c r="D95" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E95" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F95" t="s">
         <v>644</v>
@@ -6257,7 +6257,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B96" t="s">
         <v>8</v>
@@ -6266,10 +6266,10 @@
         <v>17</v>
       </c>
       <c r="D96" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E96" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F96" t="s">
         <v>644</v>
@@ -6280,7 +6280,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B97" t="s">
         <v>8</v>
@@ -6289,10 +6289,10 @@
         <v>17</v>
       </c>
       <c r="D97" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E97" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F97" t="s">
         <v>644</v>
@@ -6303,7 +6303,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B98" t="s">
         <v>8</v>
@@ -6312,10 +6312,10 @@
         <v>17</v>
       </c>
       <c r="D98" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E98" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F98" t="s">
         <v>644</v>
@@ -6326,7 +6326,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B99" t="s">
         <v>8</v>
@@ -6335,10 +6335,10 @@
         <v>17</v>
       </c>
       <c r="D99" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E99" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F99" t="s">
         <v>644</v>
@@ -6349,7 +6349,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B100" t="s">
         <v>8</v>
@@ -6358,10 +6358,10 @@
         <v>17</v>
       </c>
       <c r="D100" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E100" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F100" t="s">
         <v>644</v>
@@ -6372,7 +6372,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B101" t="s">
         <v>8</v>
@@ -6381,10 +6381,10 @@
         <v>17</v>
       </c>
       <c r="D101" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E101" t="s">
-        <v>210</v>
+        <v>537</v>
       </c>
       <c r="F101" t="s">
         <v>644</v>
@@ -6395,7 +6395,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B102" t="s">
         <v>8</v>
@@ -6404,10 +6404,10 @@
         <v>17</v>
       </c>
       <c r="D102" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="E102" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="F102" t="s">
         <v>644</v>
@@ -6418,7 +6418,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B103" t="s">
         <v>8</v>
@@ -6427,10 +6427,10 @@
         <v>17</v>
       </c>
       <c r="D103" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E103" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F103" t="s">
         <v>644</v>
@@ -6441,7 +6441,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B104" t="s">
         <v>8</v>
@@ -6450,10 +6450,10 @@
         <v>17</v>
       </c>
       <c r="D104" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="E104" t="s">
-        <v>540</v>
+        <v>210</v>
       </c>
       <c r="F104" t="s">
         <v>644</v>
@@ -6464,7 +6464,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B105" t="s">
         <v>8</v>
@@ -6473,10 +6473,10 @@
         <v>17</v>
       </c>
       <c r="D105" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E105" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F105" t="s">
         <v>644</v>
@@ -6487,7 +6487,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B106" t="s">
         <v>8</v>
@@ -6496,10 +6496,10 @@
         <v>17</v>
       </c>
       <c r="D106" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E106" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F106" t="s">
         <v>644</v>
@@ -6510,7 +6510,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B107" t="s">
         <v>8</v>
@@ -6519,10 +6519,10 @@
         <v>17</v>
       </c>
       <c r="D107" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E107" t="s">
-        <v>222</v>
+        <v>542</v>
       </c>
       <c r="F107" t="s">
         <v>644</v>
@@ -6533,7 +6533,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B108" t="s">
         <v>8</v>
@@ -6542,10 +6542,10 @@
         <v>17</v>
       </c>
       <c r="D108" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E108" t="s">
-        <v>543</v>
+        <v>222</v>
       </c>
       <c r="F108" t="s">
         <v>644</v>
@@ -6556,7 +6556,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B109" t="s">
         <v>8</v>
@@ -6565,10 +6565,10 @@
         <v>17</v>
       </c>
       <c r="D109" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E109" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F109" t="s">
         <v>644</v>
@@ -6602,7 +6602,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B111" t="s">
         <v>8</v>
@@ -6611,10 +6611,10 @@
         <v>17</v>
       </c>
       <c r="D111" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E111" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F111" t="s">
         <v>644</v>
@@ -6625,7 +6625,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B112" t="s">
         <v>8</v>
@@ -6634,10 +6634,10 @@
         <v>17</v>
       </c>
       <c r="D112" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E112" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F112" t="s">
         <v>644</v>
@@ -6648,7 +6648,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B113" t="s">
         <v>8</v>
@@ -6657,10 +6657,10 @@
         <v>17</v>
       </c>
       <c r="D113" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E113" t="s">
-        <v>234</v>
+        <v>547</v>
       </c>
       <c r="F113" t="s">
         <v>644</v>
@@ -6671,7 +6671,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B114" t="s">
         <v>8</v>
@@ -6680,10 +6680,10 @@
         <v>17</v>
       </c>
       <c r="D114" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E114" t="s">
-        <v>236</v>
+        <v>548</v>
       </c>
       <c r="F114" t="s">
         <v>644</v>
@@ -6694,7 +6694,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B115" t="s">
         <v>8</v>
@@ -6703,10 +6703,10 @@
         <v>17</v>
       </c>
       <c r="D115" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E115" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F115" t="s">
         <v>644</v>
@@ -6717,7 +6717,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B116" t="s">
         <v>8</v>
@@ -6726,10 +6726,10 @@
         <v>17</v>
       </c>
       <c r="D116" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="E116" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="F116" t="s">
         <v>644</v>
@@ -6740,7 +6740,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B117" t="s">
         <v>8</v>
@@ -6749,10 +6749,10 @@
         <v>17</v>
       </c>
       <c r="D117" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E117" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="F117" t="s">
         <v>644</v>
@@ -6763,7 +6763,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B118" t="s">
         <v>8</v>
@@ -6772,10 +6772,10 @@
         <v>17</v>
       </c>
       <c r="D118" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E118" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="F118" t="s">
         <v>644</v>
@@ -6786,7 +6786,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B119" t="s">
         <v>8</v>
@@ -6795,10 +6795,10 @@
         <v>17</v>
       </c>
       <c r="D119" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E119" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F119" t="s">
         <v>644</v>
@@ -6809,7 +6809,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B120" t="s">
         <v>8</v>
@@ -6818,10 +6818,10 @@
         <v>17</v>
       </c>
       <c r="D120" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E120" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="F120" t="s">
         <v>644</v>
@@ -6832,7 +6832,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B121" t="s">
         <v>8</v>
@@ -6841,10 +6841,10 @@
         <v>17</v>
       </c>
       <c r="D121" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E121" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="F121" t="s">
         <v>644</v>
@@ -6855,7 +6855,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B122" t="s">
         <v>8</v>
@@ -6864,10 +6864,10 @@
         <v>17</v>
       </c>
       <c r="D122" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E122" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="F122" t="s">
         <v>644</v>
@@ -6878,7 +6878,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B123" t="s">
         <v>8</v>
@@ -6887,10 +6887,10 @@
         <v>17</v>
       </c>
       <c r="D123" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E123" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F123" t="s">
         <v>644</v>
@@ -6901,7 +6901,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B124" t="s">
         <v>8</v>
@@ -6910,10 +6910,10 @@
         <v>17</v>
       </c>
       <c r="D124" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E124" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="F124" t="s">
         <v>644</v>
@@ -6924,7 +6924,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B125" t="s">
         <v>8</v>
@@ -6933,10 +6933,10 @@
         <v>17</v>
       </c>
       <c r="D125" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E125" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="F125" t="s">
         <v>644</v>
@@ -6947,7 +6947,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="B126" t="s">
         <v>8</v>
@@ -6956,10 +6956,10 @@
         <v>17</v>
       </c>
       <c r="D126" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="E126" t="s">
-        <v>559</v>
+        <v>234</v>
       </c>
       <c r="F126" t="s">
         <v>644</v>
@@ -6970,7 +6970,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="B127" t="s">
         <v>8</v>
@@ -6979,10 +6979,10 @@
         <v>17</v>
       </c>
       <c r="D127" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="E127" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="F127" t="s">
         <v>644</v>
@@ -6993,7 +6993,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B128" t="s">
         <v>8</v>
@@ -7002,10 +7002,10 @@
         <v>17</v>
       </c>
       <c r="D128" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E128" t="s">
-        <v>560</v>
+        <v>261</v>
       </c>
       <c r="F128" t="s">
         <v>644</v>
@@ -7016,7 +7016,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B129" t="s">
         <v>8</v>
@@ -7025,10 +7025,10 @@
         <v>17</v>
       </c>
       <c r="D129" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E129" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F129" t="s">
         <v>644</v>
@@ -7039,7 +7039,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B130" t="s">
         <v>8</v>
@@ -7048,10 +7048,10 @@
         <v>17</v>
       </c>
       <c r="D130" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E130" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F130" t="s">
         <v>644</v>
@@ -7062,7 +7062,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B131" t="s">
         <v>8</v>
@@ -7071,10 +7071,10 @@
         <v>17</v>
       </c>
       <c r="D131" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E131" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F131" t="s">
         <v>644</v>
@@ -7085,7 +7085,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B132" t="s">
         <v>8</v>
@@ -7094,10 +7094,10 @@
         <v>17</v>
       </c>
       <c r="D132" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E132" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F132" t="s">
         <v>644</v>
@@ -7108,7 +7108,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B133" t="s">
         <v>8</v>
@@ -7117,10 +7117,10 @@
         <v>17</v>
       </c>
       <c r="D133" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E133" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F133" t="s">
         <v>644</v>
@@ -7131,7 +7131,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B134" t="s">
         <v>8</v>
@@ -7140,10 +7140,10 @@
         <v>17</v>
       </c>
       <c r="D134" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E134" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F134" t="s">
         <v>644</v>
@@ -7154,7 +7154,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B135" t="s">
         <v>8</v>
@@ -7163,10 +7163,10 @@
         <v>17</v>
       </c>
       <c r="D135" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E135" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F135" t="s">
         <v>644</v>
@@ -7189,7 +7189,7 @@
         <v>277</v>
       </c>
       <c r="E136" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F136" t="s">
         <v>644</v>
@@ -7200,7 +7200,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B137" t="s">
         <v>8</v>
@@ -7209,10 +7209,10 @@
         <v>17</v>
       </c>
       <c r="D137" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E137" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F137" t="s">
         <v>644</v>
@@ -7223,7 +7223,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B138" t="s">
         <v>8</v>
@@ -7232,10 +7232,10 @@
         <v>17</v>
       </c>
       <c r="D138" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E138" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F138" t="s">
         <v>644</v>
@@ -7246,7 +7246,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B139" t="s">
         <v>8</v>
@@ -7255,10 +7255,10 @@
         <v>17</v>
       </c>
       <c r="D139" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E139" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F139" t="s">
         <v>644</v>
@@ -7269,7 +7269,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B140" t="s">
         <v>8</v>
@@ -7278,10 +7278,10 @@
         <v>17</v>
       </c>
       <c r="D140" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E140" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F140" t="s">
         <v>644</v>
@@ -7292,7 +7292,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B141" t="s">
         <v>8</v>
@@ -7301,10 +7301,10 @@
         <v>17</v>
       </c>
       <c r="D141" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E141" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F141" t="s">
         <v>644</v>
@@ -7315,7 +7315,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B142" t="s">
         <v>8</v>
@@ -7324,10 +7324,10 @@
         <v>17</v>
       </c>
       <c r="D142" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E142" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F142" t="s">
         <v>644</v>
@@ -7338,7 +7338,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B143" t="s">
         <v>8</v>
@@ -7347,10 +7347,10 @@
         <v>17</v>
       </c>
       <c r="D143" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E143" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F143" t="s">
         <v>644</v>
@@ -7361,7 +7361,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B144" t="s">
         <v>8</v>
@@ -7370,10 +7370,10 @@
         <v>17</v>
       </c>
       <c r="D144" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E144" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F144" t="s">
         <v>644</v>
@@ -7384,7 +7384,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B145" t="s">
         <v>8</v>
@@ -7393,10 +7393,10 @@
         <v>17</v>
       </c>
       <c r="D145" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E145" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F145" t="s">
         <v>644</v>
@@ -7407,7 +7407,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B146" t="s">
         <v>8</v>
@@ -7416,10 +7416,10 @@
         <v>17</v>
       </c>
       <c r="D146" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E146" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F146" t="s">
         <v>644</v>
@@ -7430,7 +7430,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B147" t="s">
         <v>8</v>
@@ -7439,10 +7439,10 @@
         <v>17</v>
       </c>
       <c r="D147" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E147" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F147" t="s">
         <v>644</v>
@@ -7453,7 +7453,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B148" t="s">
         <v>8</v>
@@ -7462,10 +7462,10 @@
         <v>17</v>
       </c>
       <c r="D148" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E148" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F148" t="s">
         <v>644</v>
@@ -7476,7 +7476,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B149" t="s">
         <v>8</v>
@@ -7485,10 +7485,10 @@
         <v>17</v>
       </c>
       <c r="D149" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E149" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F149" t="s">
         <v>644</v>
@@ -7499,7 +7499,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B150" t="s">
         <v>8</v>
@@ -7508,10 +7508,10 @@
         <v>17</v>
       </c>
       <c r="D150" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E150" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F150" t="s">
         <v>644</v>
@@ -7522,7 +7522,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B151" t="s">
         <v>8</v>
@@ -7531,10 +7531,10 @@
         <v>17</v>
       </c>
       <c r="D151" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E151" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F151" t="s">
         <v>644</v>
@@ -7545,7 +7545,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B152" t="s">
         <v>8</v>
@@ -7554,10 +7554,10 @@
         <v>17</v>
       </c>
       <c r="D152" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E152" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F152" t="s">
         <v>644</v>
@@ -7568,7 +7568,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B153" t="s">
         <v>8</v>
@@ -7580,7 +7580,7 @@
         <v>308</v>
       </c>
       <c r="E153" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F153" t="s">
         <v>644</v>
@@ -7591,7 +7591,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B154" t="s">
         <v>8</v>
@@ -7600,10 +7600,10 @@
         <v>17</v>
       </c>
       <c r="D154" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E154" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F154" t="s">
         <v>644</v>
@@ -7614,7 +7614,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B155" t="s">
         <v>8</v>
@@ -7623,10 +7623,10 @@
         <v>17</v>
       </c>
       <c r="D155" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E155" t="s">
-        <v>313</v>
+        <v>586</v>
       </c>
       <c r="F155" t="s">
         <v>644</v>
@@ -7729,7 +7729,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B160" t="s">
         <v>8</v>
@@ -7738,10 +7738,10 @@
         <v>17</v>
       </c>
       <c r="D160" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="E160" t="s">
-        <v>590</v>
+        <v>313</v>
       </c>
       <c r="F160" t="s">
         <v>644</v>
@@ -7752,7 +7752,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B161" t="s">
         <v>8</v>
@@ -7761,10 +7761,10 @@
         <v>17</v>
       </c>
       <c r="D161" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E161" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F161" t="s">
         <v>644</v>
@@ -7775,7 +7775,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B162" t="s">
         <v>8</v>
@@ -7784,10 +7784,10 @@
         <v>17</v>
       </c>
       <c r="D162" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E162" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F162" t="s">
         <v>644</v>
@@ -7821,7 +7821,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B164" t="s">
         <v>8</v>
@@ -7830,10 +7830,10 @@
         <v>17</v>
       </c>
       <c r="D164" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E164" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F164" t="s">
         <v>644</v>
@@ -7844,7 +7844,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B165" t="s">
         <v>8</v>
@@ -7853,10 +7853,10 @@
         <v>17</v>
       </c>
       <c r="D165" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E165" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F165" t="s">
         <v>644</v>
@@ -7867,7 +7867,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B166" t="s">
         <v>8</v>
@@ -7876,10 +7876,10 @@
         <v>17</v>
       </c>
       <c r="D166" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E166" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F166" t="s">
         <v>644</v>
@@ -7890,7 +7890,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B167" t="s">
         <v>8</v>
@@ -7899,10 +7899,10 @@
         <v>17</v>
       </c>
       <c r="D167" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E167" t="s">
-        <v>335</v>
+        <v>596</v>
       </c>
       <c r="F167" t="s">
         <v>644</v>
@@ -7913,7 +7913,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B168" t="s">
         <v>8</v>
@@ -7922,10 +7922,10 @@
         <v>17</v>
       </c>
       <c r="D168" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E168" t="s">
-        <v>597</v>
+        <v>335</v>
       </c>
       <c r="F168" t="s">
         <v>644</v>
@@ -7936,7 +7936,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B169" t="s">
         <v>8</v>
@@ -7945,10 +7945,10 @@
         <v>17</v>
       </c>
       <c r="D169" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E169" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F169" t="s">
         <v>644</v>
@@ -7959,7 +7959,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B170" t="s">
         <v>8</v>
@@ -7968,10 +7968,10 @@
         <v>17</v>
       </c>
       <c r="D170" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E170" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F170" t="s">
         <v>644</v>
@@ -8005,7 +8005,7 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B172" t="s">
         <v>8</v>
@@ -8014,10 +8014,10 @@
         <v>17</v>
       </c>
       <c r="D172" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E172" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="F172" t="s">
         <v>644</v>
@@ -8028,7 +8028,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B173" t="s">
         <v>8</v>
@@ -8037,10 +8037,10 @@
         <v>17</v>
       </c>
       <c r="D173" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E173" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F173" t="s">
         <v>644</v>
@@ -8051,7 +8051,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B174" t="s">
         <v>8</v>
@@ -8060,10 +8060,10 @@
         <v>17</v>
       </c>
       <c r="D174" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E174" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F174" t="s">
         <v>644</v>
@@ -8074,7 +8074,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B175" t="s">
         <v>8</v>
@@ -8083,10 +8083,10 @@
         <v>17</v>
       </c>
       <c r="D175" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E175" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F175" t="s">
         <v>644</v>
@@ -8097,7 +8097,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B176" t="s">
         <v>8</v>
@@ -8106,10 +8106,10 @@
         <v>17</v>
       </c>
       <c r="D176" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E176" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F176" t="s">
         <v>644</v>
@@ -8120,7 +8120,7 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B177" t="s">
         <v>8</v>
@@ -8129,10 +8129,10 @@
         <v>17</v>
       </c>
       <c r="D177" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E177" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F177" t="s">
         <v>644</v>
@@ -8143,7 +8143,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B178" t="s">
         <v>8</v>
@@ -8152,10 +8152,10 @@
         <v>17</v>
       </c>
       <c r="D178" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E178" t="s">
-        <v>357</v>
+        <v>606</v>
       </c>
       <c r="F178" t="s">
         <v>644</v>
@@ -8304,7 +8304,7 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="B185" t="s">
         <v>8</v>
@@ -8313,10 +8313,10 @@
         <v>17</v>
       </c>
       <c r="D185" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="E185" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="F185" t="s">
         <v>644</v>
@@ -8327,7 +8327,7 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B186" t="s">
         <v>8</v>
@@ -8336,10 +8336,10 @@
         <v>17</v>
       </c>
       <c r="D186" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E186" t="s">
-        <v>611</v>
+        <v>371</v>
       </c>
       <c r="F186" t="s">
         <v>644</v>
@@ -8350,7 +8350,7 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B187" t="s">
         <v>8</v>
@@ -8359,10 +8359,10 @@
         <v>17</v>
       </c>
       <c r="D187" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E187" t="s">
-        <v>375</v>
+        <v>611</v>
       </c>
       <c r="F187" t="s">
         <v>644</v>
@@ -8373,7 +8373,7 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B188" t="s">
         <v>8</v>
@@ -8382,10 +8382,10 @@
         <v>17</v>
       </c>
       <c r="D188" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E188" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F188" t="s">
         <v>644</v>
@@ -8672,7 +8672,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B201" t="s">
         <v>8</v>
@@ -8681,10 +8681,10 @@
         <v>17</v>
       </c>
       <c r="D201" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E201" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="F201" t="s">
         <v>644</v>
@@ -8695,7 +8695,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B202" t="s">
         <v>8</v>
@@ -8704,10 +8704,10 @@
         <v>17</v>
       </c>
       <c r="D202" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E202" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F202" t="s">
         <v>644</v>
@@ -8879,7 +8879,7 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B210" t="s">
         <v>8</v>
@@ -8888,10 +8888,10 @@
         <v>17</v>
       </c>
       <c r="D210" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="E210" t="s">
-        <v>421</v>
+        <v>630</v>
       </c>
       <c r="F210" t="s">
         <v>644</v>
@@ -8902,7 +8902,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B211" t="s">
         <v>8</v>
@@ -8911,10 +8911,10 @@
         <v>17</v>
       </c>
       <c r="D211" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E211" t="s">
-        <v>630</v>
+        <v>421</v>
       </c>
       <c r="F211" t="s">
         <v>644</v>
@@ -9177,6 +9177,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:G222">
+    <sortCondition ref="A2:A222"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9186,7 +9189,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A41"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9228,7 +9231,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -9277,7 +9280,7 @@
         <v>684</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -9300,7 +9303,7 @@
         <v>708</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G5">
         <v>150</v>
@@ -9346,7 +9349,7 @@
         <v>710</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G7">
         <v>150</v>
@@ -9745,7 +9748,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>666</v>
+        <v>670</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -9754,10 +9757,10 @@
         <v>683</v>
       </c>
       <c r="D25" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="E25" t="s">
-        <v>728</v>
+        <v>700</v>
       </c>
       <c r="F25" t="s">
         <v>644</v>
@@ -9768,7 +9771,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>667</v>
+        <v>671</v>
       </c>
       <c r="B26" t="s">
         <v>8</v>
@@ -9777,10 +9780,10 @@
         <v>683</v>
       </c>
       <c r="D26" t="s">
-        <v>698</v>
+        <v>683</v>
       </c>
       <c r="E26" t="s">
-        <v>729</v>
+        <v>683</v>
       </c>
       <c r="F26" t="s">
         <v>644</v>
@@ -9791,7 +9794,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -9800,10 +9803,10 @@
         <v>683</v>
       </c>
       <c r="D27" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="E27" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="F27" t="s">
         <v>644</v>
@@ -9814,7 +9817,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -9823,10 +9826,10 @@
         <v>683</v>
       </c>
       <c r="D28" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E28" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F28" t="s">
         <v>644</v>
@@ -9837,7 +9840,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -9846,10 +9849,10 @@
         <v>683</v>
       </c>
       <c r="D29" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E29" t="s">
-        <v>700</v>
+        <v>730</v>
       </c>
       <c r="F29" t="s">
         <v>644</v>
@@ -9860,7 +9863,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
@@ -9869,10 +9872,10 @@
         <v>683</v>
       </c>
       <c r="D30" t="s">
-        <v>683</v>
+        <v>699</v>
       </c>
       <c r="E30" t="s">
-        <v>683</v>
+        <v>731</v>
       </c>
       <c r="F30" t="s">
         <v>644</v>
@@ -10135,6 +10138,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:G41">
+    <sortCondition ref="A2:A41"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -10144,8 +10150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10187,7 +10193,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -10236,7 +10242,7 @@
         <v>800</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -10259,7 +10265,7 @@
         <v>801</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G5">
         <v>150</v>
@@ -10305,7 +10311,7 @@
         <v>803</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G7">
         <v>150</v>
@@ -11102,8 +11108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11145,7 +11151,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -11194,7 +11200,7 @@
         <v>878</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -11217,7 +11223,7 @@
         <v>879</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G5">
         <v>150</v>
@@ -11263,7 +11269,7 @@
         <v>881</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G7">
         <v>150</v>
@@ -11593,7 +11599,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -11602,10 +11608,10 @@
         <v>874</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
+        <v>874</v>
       </c>
       <c r="E22" t="s">
-        <v>896</v>
+        <v>874</v>
       </c>
       <c r="F22" t="s">
         <v>644</v>
@@ -11616,7 +11622,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -11625,10 +11631,10 @@
         <v>874</v>
       </c>
       <c r="D23" t="s">
-        <v>790</v>
+        <v>206</v>
       </c>
       <c r="E23" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="F23" t="s">
         <v>644</v>
@@ -11639,7 +11645,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -11648,10 +11654,10 @@
         <v>874</v>
       </c>
       <c r="D24" t="s">
-        <v>216</v>
+        <v>790</v>
       </c>
       <c r="E24" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F24" t="s">
         <v>644</v>
@@ -11662,7 +11668,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -11671,10 +11677,10 @@
         <v>874</v>
       </c>
       <c r="D25" t="s">
-        <v>874</v>
+        <v>216</v>
       </c>
       <c r="E25" t="s">
-        <v>874</v>
+        <v>898</v>
       </c>
       <c r="F25" t="s">
         <v>644</v>
@@ -11708,7 +11714,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -11717,10 +11723,10 @@
         <v>874</v>
       </c>
       <c r="D27" t="s">
-        <v>699</v>
+        <v>877</v>
       </c>
       <c r="E27" t="s">
-        <v>900</v>
+        <v>877</v>
       </c>
       <c r="F27" t="s">
         <v>644</v>
@@ -11731,7 +11737,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -11743,7 +11749,7 @@
         <v>699</v>
       </c>
       <c r="E28" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F28" t="s">
         <v>644</v>
@@ -11754,7 +11760,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -11763,10 +11769,10 @@
         <v>874</v>
       </c>
       <c r="D29" t="s">
-        <v>877</v>
+        <v>699</v>
       </c>
       <c r="E29" t="s">
-        <v>877</v>
+        <v>901</v>
       </c>
       <c r="F29" t="s">
         <v>644</v>
@@ -12029,6 +12035,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A5:G40">
+    <sortCondition ref="A5:A40"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12037,8 +12046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12080,7 +12089,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -12114,7 +12123,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -12123,13 +12132,13 @@
         <v>955</v>
       </c>
       <c r="D4" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="E4" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -12137,7 +12146,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -12146,13 +12155,13 @@
         <v>955</v>
       </c>
       <c r="D5" t="s">
-        <v>957</v>
+        <v>685</v>
       </c>
       <c r="E5" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G5">
         <v>150</v>
@@ -12160,7 +12169,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -12169,10 +12178,10 @@
         <v>955</v>
       </c>
       <c r="D6" t="s">
-        <v>685</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="F6" t="s">
         <v>644</v>
@@ -12183,7 +12192,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -12192,13 +12201,13 @@
         <v>955</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>687</v>
       </c>
       <c r="E7" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G7">
         <v>150</v>
@@ -12206,7 +12215,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -12215,10 +12224,10 @@
         <v>955</v>
       </c>
       <c r="D8" t="s">
-        <v>687</v>
+        <v>958</v>
       </c>
       <c r="E8" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="F8" t="s">
         <v>644</v>
@@ -12229,7 +12238,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -12238,10 +12247,10 @@
         <v>955</v>
       </c>
       <c r="D9" t="s">
-        <v>958</v>
+        <v>688</v>
       </c>
       <c r="E9" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="F9" t="s">
         <v>644</v>
@@ -12252,7 +12261,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -12261,10 +12270,10 @@
         <v>955</v>
       </c>
       <c r="D10" t="s">
-        <v>688</v>
+        <v>86</v>
       </c>
       <c r="E10" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="F10" t="s">
         <v>644</v>
@@ -12275,7 +12284,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -12284,10 +12293,10 @@
         <v>955</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="F11" t="s">
         <v>644</v>
@@ -12298,7 +12307,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -12307,10 +12316,10 @@
         <v>955</v>
       </c>
       <c r="D12" t="s">
-        <v>94</v>
+        <v>959</v>
       </c>
       <c r="E12" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="F12" t="s">
         <v>644</v>
@@ -12321,7 +12330,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -12330,10 +12339,10 @@
         <v>955</v>
       </c>
       <c r="D13" t="s">
-        <v>959</v>
+        <v>690</v>
       </c>
       <c r="E13" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="F13" t="s">
         <v>644</v>
@@ -12344,7 +12353,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -12353,10 +12362,10 @@
         <v>955</v>
       </c>
       <c r="D14" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E14" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="F14" t="s">
         <v>644</v>
@@ -12367,7 +12376,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -12376,10 +12385,10 @@
         <v>955</v>
       </c>
       <c r="D15" t="s">
-        <v>691</v>
+        <v>960</v>
       </c>
       <c r="E15" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="F15" t="s">
         <v>644</v>
@@ -12390,7 +12399,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -12399,10 +12408,10 @@
         <v>955</v>
       </c>
       <c r="D16" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="E16" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="F16" t="s">
         <v>644</v>
@@ -12413,7 +12422,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -12422,10 +12431,10 @@
         <v>955</v>
       </c>
       <c r="D17" t="s">
-        <v>961</v>
+        <v>135</v>
       </c>
       <c r="E17" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="F17" t="s">
         <v>644</v>
@@ -12436,7 +12445,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -12445,10 +12454,10 @@
         <v>955</v>
       </c>
       <c r="D18" t="s">
-        <v>135</v>
+        <v>962</v>
       </c>
       <c r="E18" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="F18" t="s">
         <v>644</v>
@@ -12459,7 +12468,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -12468,10 +12477,10 @@
         <v>955</v>
       </c>
       <c r="D19" t="s">
-        <v>962</v>
+        <v>929</v>
       </c>
       <c r="E19" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="F19" t="s">
         <v>644</v>
@@ -12482,7 +12491,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B20" t="s">
         <v>8</v>
@@ -12491,10 +12500,10 @@
         <v>955</v>
       </c>
       <c r="D20" t="s">
-        <v>929</v>
+        <v>789</v>
       </c>
       <c r="E20" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="F20" t="s">
         <v>644</v>
@@ -12505,7 +12514,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -12514,10 +12523,10 @@
         <v>955</v>
       </c>
       <c r="D21" t="s">
-        <v>789</v>
+        <v>216</v>
       </c>
       <c r="E21" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="F21" t="s">
         <v>644</v>
@@ -12551,7 +12560,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
@@ -12560,10 +12569,10 @@
         <v>955</v>
       </c>
       <c r="D23" t="s">
-        <v>216</v>
+        <v>876</v>
       </c>
       <c r="E23" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="F23" t="s">
         <v>644</v>
@@ -12574,7 +12583,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
@@ -12583,10 +12592,10 @@
         <v>955</v>
       </c>
       <c r="D24" t="s">
-        <v>876</v>
+        <v>963</v>
       </c>
       <c r="E24" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="F24" t="s">
         <v>644</v>
@@ -12597,7 +12606,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>934</v>
+        <v>938</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
@@ -12606,10 +12615,10 @@
         <v>955</v>
       </c>
       <c r="D25" t="s">
-        <v>963</v>
+        <v>955</v>
       </c>
       <c r="E25" t="s">
-        <v>994</v>
+        <v>955</v>
       </c>
       <c r="F25" t="s">
         <v>644</v>
@@ -12689,7 +12698,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>938</v>
+        <v>913</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
@@ -12698,13 +12707,13 @@
         <v>955</v>
       </c>
       <c r="D29" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="E29" t="s">
-        <v>955</v>
+        <v>973</v>
       </c>
       <c r="F29" t="s">
-        <v>644</v>
+        <v>9</v>
       </c>
       <c r="G29">
         <v>150</v>
@@ -12758,7 +12767,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="B32" t="s">
         <v>8</v>
@@ -12767,10 +12776,10 @@
         <v>955</v>
       </c>
       <c r="D32" t="s">
-        <v>702</v>
+        <v>966</v>
       </c>
       <c r="E32" t="s">
-        <v>1000</v>
+        <v>966</v>
       </c>
       <c r="F32" t="s">
         <v>644</v>
@@ -12781,7 +12790,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
@@ -12790,10 +12799,10 @@
         <v>955</v>
       </c>
       <c r="D33" t="s">
-        <v>795</v>
+        <v>702</v>
       </c>
       <c r="E33" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="F33" t="s">
         <v>644</v>
@@ -12804,7 +12813,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B34" t="s">
         <v>8</v>
@@ -12813,10 +12822,10 @@
         <v>955</v>
       </c>
       <c r="D34" t="s">
-        <v>966</v>
+        <v>795</v>
       </c>
       <c r="E34" t="s">
-        <v>966</v>
+        <v>1001</v>
       </c>
       <c r="F34" t="s">
         <v>644</v>
@@ -12942,7 +12951,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B40" t="s">
         <v>8</v>
@@ -12951,10 +12960,10 @@
         <v>955</v>
       </c>
       <c r="D40" t="s">
-        <v>707</v>
+        <v>970</v>
       </c>
       <c r="E40" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="F40" t="s">
         <v>644</v>
@@ -12965,7 +12974,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B41" t="s">
         <v>8</v>
@@ -12974,10 +12983,10 @@
         <v>955</v>
       </c>
       <c r="D41" t="s">
-        <v>799</v>
+        <v>707</v>
       </c>
       <c r="E41" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="F41" t="s">
         <v>644</v>
@@ -12988,7 +12997,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B42" t="s">
         <v>8</v>
@@ -12997,10 +13006,10 @@
         <v>955</v>
       </c>
       <c r="D42" t="s">
-        <v>970</v>
+        <v>799</v>
       </c>
       <c r="E42" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="F42" t="s">
         <v>644</v>
@@ -13079,6 +13088,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A4:G45">
+    <sortCondition ref="A4:A45"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13087,8 +13099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="A1:G22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13130,7 +13142,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -13179,7 +13191,7 @@
         <v>1047</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -13202,7 +13214,7 @@
         <v>1048</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G5">
         <v>150</v>
@@ -13248,7 +13260,7 @@
         <v>1050</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G7">
         <v>150</v>
@@ -13555,7 +13567,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
@@ -13567,7 +13579,7 @@
         <v>1046</v>
       </c>
       <c r="E21" t="s">
-        <v>1046</v>
+        <v>1063</v>
       </c>
       <c r="F21" t="s">
         <v>644</v>
@@ -13578,7 +13590,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
@@ -13590,7 +13602,7 @@
         <v>1046</v>
       </c>
       <c r="E22" t="s">
-        <v>1063</v>
+        <v>1046</v>
       </c>
       <c r="F22" t="s">
         <v>644</v>
@@ -13600,6 +13612,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A4:G22">
+    <sortCondition ref="A4:A22"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13608,8 +13623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13651,7 +13666,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -13700,7 +13715,7 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G4">
         <v>150</v>
@@ -13723,7 +13738,7 @@
         <v>683</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G5">
         <v>150</v>
@@ -13769,7 +13784,7 @@
         <v>874</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>644</v>
       </c>
       <c r="G7">
         <v>150</v>

</xml_diff>

<commit_message>
Atlantic Coast Conf team order
this element was used as the header and so did not get put into the sort
order correctly. It has been fixed.
</commit_message>
<xml_diff>
--- a/filters/db/teams-by-league.xlsx
+++ b/filters/db/teams-by-league.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="8520" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="20115" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="NCAA" sheetId="1" r:id="rId1"/>
@@ -4064,8 +4064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G222"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4141,7 +4141,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -4150,10 +4150,10 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>446</v>
       </c>
       <c r="F4" t="s">
         <v>644</v>
@@ -4164,7 +4164,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -4173,10 +4173,10 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F5" t="s">
         <v>644</v>
@@ -4187,7 +4187,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -4196,10 +4196,10 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F6" t="s">
         <v>644</v>
@@ -4210,7 +4210,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -4219,10 +4219,10 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F7" t="s">
         <v>644</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -4242,10 +4242,10 @@
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F8" t="s">
         <v>644</v>
@@ -4256,7 +4256,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -4265,10 +4265,10 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F9" t="s">
         <v>644</v>
@@ -4279,7 +4279,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -4288,10 +4288,10 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="F10" t="s">
         <v>644</v>
@@ -4302,7 +4302,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -4311,10 +4311,10 @@
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F11" t="s">
         <v>644</v>
@@ -4325,7 +4325,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -4334,10 +4334,10 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="F12" t="s">
         <v>644</v>
@@ -4348,7 +4348,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -4357,10 +4357,10 @@
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F13" t="s">
         <v>644</v>
@@ -4371,7 +4371,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -4380,10 +4380,10 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>455</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
         <v>644</v>
@@ -9177,8 +9177,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G222">
-    <sortCondition ref="A2:A222"/>
+  <sortState ref="A4:G222">
+    <sortCondition ref="A4:A222"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10150,7 +10150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>